<commit_message>
add test cases for Geometric Asian Options
</commit_message>
<xml_diff>
--- a/hand-calculation/OptionPricingCal.xlsx
+++ b/hand-calculation/OptionPricingCal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wachi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wachi\Desktop\PyOptionPricing\hand-calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C8CF6-E515-41B9-9ED5-958D17D8FB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDFB3E-E78D-42D1-80E3-4D7BD3F44935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>S0</t>
   </si>
@@ -137,6 +137,12 @@
   <si>
     <t>nu</t>
   </si>
+  <si>
+    <t>Arithmetic Asian</t>
+  </si>
+  <si>
+    <t>Geometric Asian</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +200,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -237,20 +255,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
+    <cellStyle name="60% - Accent4" xfId="5" builtinId="44"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="A15:B22"/>
+      <selection activeCell="X13" sqref="Q1:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,15 +567,27 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
@@ -560,8 +596,24 @@
         <v>20</v>
       </c>
       <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="4"/>
+      <c r="U2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -610,8 +662,32 @@
       <c r="P3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -634,7 +710,7 @@
       </c>
       <c r="G4" s="1">
         <f>($B$21^E4)*($B$22^F4)</f>
-        <v>9.1125000000000039E-2</v>
+        <v>0.125</v>
       </c>
       <c r="H4" s="1">
         <f>$B$15</f>
@@ -661,19 +737,51 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <f>$G4*M4</f>
+        <f t="shared" ref="N4:N11" si="0">$G4*M4</f>
         <v>0</v>
       </c>
       <c r="O4" s="2">
         <f>MAX(0,$B$19-K4)</f>
-        <v>57.099999999999994</v>
+        <v>37.099999999999994</v>
       </c>
       <c r="P4" s="2">
-        <f>$G4*O4</f>
-        <v>5.203237500000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="P4:P11" si="1">$G4*O4</f>
+        <v>4.6374999999999993</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>MAX(AVERAGE(I4:K4)-$B$19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <f>$G4*Q4</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <f>MAX(0,$B$19-L4)</f>
+        <v>28.700000000000003</v>
+      </c>
+      <c r="T4" s="4">
+        <f>$G4*S4</f>
+        <v>3.5875000000000004</v>
+      </c>
+      <c r="U4" s="5">
+        <f>MAX(GEOMEAN(I4:K4)-$B$19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <f>$G4*U4</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <f>MAX(0,$B$19-GEOMEAN(I4:K4))</f>
+        <v>29</v>
+      </c>
+      <c r="X4" s="5">
+        <f>$G4*W4</f>
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -687,55 +795,87 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E11" si="0">COUNTIF(B5:D5,1)</f>
+        <f t="shared" ref="E5:E11" si="2">COUNTIF(B5:D5,1)</f>
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F11" si="1">COUNTIF(B5:D5,0)</f>
+        <f t="shared" ref="F5:F11" si="3">COUNTIF(B5:D5,0)</f>
         <v>2</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G11" si="2">($B$21^E5)*($B$22^F5)</f>
-        <v>0.11137500000000003</v>
+        <f t="shared" ref="G5:G11" si="4">($B$21^E5)*($B$22^F5)</f>
+        <v>0.125</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H11" si="3">$B$15</f>
+        <f t="shared" ref="H5:H11" si="5">$B$15</f>
         <v>100</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I11" si="4">H5*((1+$B$16)*B5+(1+$B$17)*(1-B5))</f>
+        <f t="shared" ref="I5:I11" si="6">H5*((1+$B$16)*B5+(1+$B$17)*(1-B5))</f>
         <v>90</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" ref="J5:J11" si="5">I5*((1+$B$16)*C5+(1+$B$17)*(1-C5))</f>
+        <f t="shared" ref="J5:J11" si="7">I5*((1+$B$16)*C5+(1+$B$17)*(1-C5))</f>
         <v>81</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" ref="K5:K11" si="6">J5*((1+$B$16)*D5+(1+$B$17)*(1-D5))</f>
+        <f t="shared" ref="K5:K11" si="8">J5*((1+$B$16)*D5+(1+$B$17)*(1-D5))</f>
         <v>89.100000000000009</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" ref="L5:L11" si="7">AVERAGE(I5:K5)</f>
+        <f t="shared" ref="L5:L11" si="9">AVERAGE(I5:K5)</f>
         <v>86.7</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M11" si="8">MAX(K5-$B$19, 0)</f>
+        <f t="shared" ref="M5:M11" si="10">MAX(K5-$B$19, 0)</f>
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <f>$G5*M5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" ref="O5:O11" si="9">MAX(0,$B$19-K5)</f>
-        <v>40.899999999999991</v>
+        <f t="shared" ref="O5:O11" si="11">MAX(0,$B$19-K5)</f>
+        <v>20.899999999999991</v>
       </c>
       <c r="P5" s="2">
-        <f>$G5*O5</f>
-        <v>4.5552375000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.6124999999999989</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>MAX(AVERAGE(I5:K5)-$B$19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" ref="R5:R11" si="12">$G5*Q5</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" ref="S5:S11" si="13">MAX(0,$B$19-L5)</f>
+        <v>23.299999999999997</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" ref="T5:T11" si="14">$G5*S5</f>
+        <v>2.9124999999999996</v>
+      </c>
+      <c r="U5" s="5">
+        <f t="shared" ref="U5:U11" si="15">MAX(GEOMEAN(I5:K5)-$B$19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="5">
+        <f t="shared" ref="V5:V11" si="16">$G5*U5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
+        <f t="shared" ref="W5:W11" si="17">MAX(0,$B$19-GEOMEAN(I5:K5))</f>
+        <v>23.396573090112682</v>
+      </c>
+      <c r="X5" s="5">
+        <f t="shared" ref="X5:X11" si="18">$G5*W5</f>
+        <v>2.9245716362640852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -749,55 +889,87 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="7"/>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="8"/>
+        <v>89.100000000000009</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="9"/>
+        <v>92.7</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="11"/>
+        <v>20.899999999999991</v>
+      </c>
+      <c r="P6" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>0.11137500000000003</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="5"/>
-        <v>99.000000000000014</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="6"/>
-        <v>89.100000000000009</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="7"/>
-        <v>92.7</v>
-      </c>
-      <c r="M6" s="2">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <f>$G6*M6</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" si="9"/>
-        <v>40.899999999999991</v>
-      </c>
-      <c r="P6" s="2">
-        <f>$G6*O6</f>
-        <v>4.5552375000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.6124999999999989</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" ref="Q5:Q11" si="19">MAX(AVERAGE(I6:K6)-$B$19, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" si="13"/>
+        <v>17.299999999999997</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="14"/>
+        <v>2.1624999999999996</v>
+      </c>
+      <c r="U6" s="5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="17"/>
+        <v>17.405511697084009</v>
+      </c>
+      <c r="X6" s="5">
+        <f t="shared" si="18"/>
+        <v>2.1756889621355011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -811,55 +983,87 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="7"/>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="8"/>
+        <v>108.90000000000002</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="9"/>
+        <v>99.300000000000011</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="11"/>
+        <v>1.0999999999999801</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.136125</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="5"/>
-        <v>99.000000000000014</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="6"/>
-        <v>108.90000000000002</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="7"/>
-        <v>99.300000000000011</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
-        <f>$G7*M7</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="9"/>
-        <v>21.09999999999998</v>
-      </c>
-      <c r="P7" s="2">
-        <f>$G7*O7</f>
-        <v>2.8722374999999971</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.13749999999999751</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="13"/>
+        <v>10.699999999999989</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="14"/>
+        <v>1.3374999999999986</v>
+      </c>
+      <c r="U7" s="5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" si="17"/>
+        <v>10.999999999999986</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" si="18"/>
+        <v>1.3749999999999982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -873,55 +1077,87 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="6"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="7"/>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="8"/>
+        <v>89.100000000000009</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="9"/>
+        <v>99.366666666666674</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="11"/>
+        <v>20.899999999999991</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="2"/>
-        <v>0.11137500000000003</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="4"/>
-        <v>110.00000000000001</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="5"/>
-        <v>99.000000000000014</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="6"/>
-        <v>89.100000000000009</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="7"/>
-        <v>99.366666666666674</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
-        <f>$G8*M8</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="9"/>
-        <v>40.899999999999991</v>
-      </c>
-      <c r="P8" s="2">
-        <f>$G8*O8</f>
-        <v>4.5552375000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.6124999999999989</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="13"/>
+        <v>10.633333333333326</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="14"/>
+        <v>1.3291666666666657</v>
+      </c>
+      <c r="U8" s="5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="17"/>
+        <v>10.999999999999986</v>
+      </c>
+      <c r="X8" s="5">
+        <f t="shared" si="18"/>
+        <v>1.3749999999999982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -935,55 +1171,87 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="6"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="7"/>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="8"/>
+        <v>108.90000000000002</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="9"/>
+        <v>105.96666666666668</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="11"/>
+        <v>1.0999999999999801</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="2"/>
-        <v>0.136125</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" si="4"/>
-        <v>110.00000000000001</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="5"/>
-        <v>99.000000000000014</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="6"/>
-        <v>108.90000000000002</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="7"/>
-        <v>105.96666666666668</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <f>$G9*M9</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="9"/>
-        <v>21.09999999999998</v>
-      </c>
-      <c r="P9" s="2">
-        <f>$G9*O9</f>
-        <v>2.8722374999999971</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.13749999999999751</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="13"/>
+        <v>4.0333333333333172</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="14"/>
+        <v>0.50416666666666465</v>
+      </c>
+      <c r="U9" s="5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="17"/>
+        <v>4.1513671101377128</v>
+      </c>
+      <c r="X9" s="5">
+        <f t="shared" si="18"/>
+        <v>0.51892088876721409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -997,55 +1265,87 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="6"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="7"/>
+        <v>121.00000000000003</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="8"/>
+        <v>108.90000000000003</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="9"/>
+        <v>113.30000000000003</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="11"/>
+        <v>1.0999999999999659</v>
+      </c>
+      <c r="P10" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.136125</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="4"/>
-        <v>110.00000000000001</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="5"/>
-        <v>121.00000000000003</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="6"/>
-        <v>108.90000000000003</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="7"/>
-        <v>113.30000000000003</v>
-      </c>
-      <c r="M10" s="2">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <f>$G10*M10</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="9"/>
-        <v>21.099999999999966</v>
-      </c>
-      <c r="P10" s="2">
-        <f>$G10*O10</f>
-        <v>2.8722374999999953</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.13749999999999574</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="19"/>
+        <v>3.3000000000000256</v>
+      </c>
+      <c r="R10" s="4">
+        <f t="shared" si="12"/>
+        <v>0.4125000000000032</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <f t="shared" si="15"/>
+        <v>3.171041259119562</v>
+      </c>
+      <c r="V10" s="5">
+        <f t="shared" si="16"/>
+        <v>0.39638015738994525</v>
+      </c>
+      <c r="W10" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1059,88 +1359,176 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="6"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="7"/>
+        <v>121.00000000000003</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="8"/>
+        <v>133.10000000000005</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="9"/>
+        <v>121.36666666666672</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="10"/>
+        <v>23.100000000000051</v>
+      </c>
+      <c r="N11" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F11" s="1">
+        <v>2.8875000000000064</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16637499999999994</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="4"/>
-        <v>110.00000000000001</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="5"/>
-        <v>121.00000000000003</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="6"/>
-        <v>133.10000000000005</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="7"/>
-        <v>121.36666666666672</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="8"/>
-        <v>3.1000000000000512</v>
-      </c>
-      <c r="N11" s="2">
-        <f>$G11*M11</f>
-        <v>0.51576250000000834</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <f>$G11*O11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="4">
+        <f t="shared" si="19"/>
+        <v>11.366666666666717</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="12"/>
+        <v>1.4208333333333396</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U11" s="5">
+        <f t="shared" si="15"/>
+        <v>11.000000000000014</v>
+      </c>
+      <c r="V11" s="5">
+        <f t="shared" si="16"/>
+        <v>1.3750000000000018</v>
+      </c>
+      <c r="W11" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N12" s="2">
         <f>SUM(N4:N11)</f>
-        <v>0.51576250000000834</v>
+        <v>2.8875000000000064</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="P12" s="2">
         <f>SUM(P4:P11)</f>
-        <v>27.485662499999989</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>12.887499999999987</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R12" s="4">
+        <f>SUM(R4:R11)</f>
+        <v>1.8333333333333428</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12" s="4">
+        <f>SUM(T4:T11)</f>
+        <v>11.833333333333329</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V12" s="5">
+        <f>SUM(V4:V11)</f>
+        <v>1.771380157389947</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X12" s="5">
+        <f>SUM(X4:X11)</f>
+        <v>11.994181487166797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N13" s="2">
         <f>N12/((1+$B$18)^3)</f>
-        <v>0.50059400117053987</v>
+        <v>2.8875000000000064</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="P13" s="2">
         <f>P12/((1+$B$18)^3)</f>
-        <v>26.677313231764302</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12.887499999999987</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R13" s="4">
+        <f>R12/((1+$B$18)^3)</f>
+        <v>1.8333333333333428</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13" s="4">
+        <f>T12/((1+$B$18)^3)</f>
+        <v>11.833333333333329</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V13" s="5">
+        <f>V12/((1+$B$18)^3)</f>
+        <v>1.771380157389947</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="X13" s="5">
+        <f>X12/((1+$B$18)^3)</f>
+        <v>11.994181487166797</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1557,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1177,7 +1565,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1578,7 @@
       </c>
       <c r="B21" s="3">
         <f>(B18-B17)/(B16-B17)</f>
-        <v>0.54999999999999993</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1199,7 +1587,7 @@
       </c>
       <c r="B22" s="3">
         <f>1-B21</f>
-        <v>0.45000000000000007</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1210,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEC0F23-5E58-4A2D-A1C8-010FDE2F7F4D}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,15 +1611,27 @@
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1240,8 +1640,24 @@
         <v>20</v>
       </c>
       <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1293,8 +1709,32 @@
       <c r="Q3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1321,10 +1761,10 @@
       </c>
       <c r="H4" s="1">
         <f>($B$44^E4)*($B$45^G4)*($B$46^F4)</f>
-        <v>2.2543738595164557E-2</v>
+        <v>1.499997657646132E-2</v>
       </c>
       <c r="I4" s="1">
-        <f>$B$34</f>
+        <f t="shared" ref="I4:I11" si="0">$B$34</f>
         <v>30</v>
       </c>
       <c r="J4" s="1">
@@ -1344,23 +1784,55 @@
         <v>18.750122600366389</v>
       </c>
       <c r="N4" s="2">
-        <f>MAX(L4-$B$38, 0)</f>
+        <f t="shared" ref="N4:N11" si="1">MAX(L4-$B$38, 0)</f>
         <v>0</v>
       </c>
       <c r="O4" s="2">
-        <f>$H4*N4</f>
+        <f t="shared" ref="O4:O11" si="2">$H4*N4</f>
         <v>0</v>
       </c>
       <c r="P4" s="2">
-        <f>MAX(0,$B$38-L4)</f>
+        <f t="shared" ref="P4:P11" si="3">MAX(0,$B$38-L4)</f>
         <v>14.612634022115024</v>
       </c>
       <c r="Q4" s="2">
-        <f>$H4*P4</f>
-        <v>0.32942340158136918</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q4:Q11" si="4">$H4*P4</f>
+        <v>0.21918916805212713</v>
+      </c>
+      <c r="R4" s="4">
+        <f>MAX(AVERAGE(J4:L4)-$B$38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
+        <f>$H4*R4</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <f>MAX(0,$B$38-M4)</f>
+        <v>10.249877399633611</v>
+      </c>
+      <c r="U4" s="4">
+        <f>$H4*T4</f>
+        <v>0.15374792090610442</v>
+      </c>
+      <c r="V4" s="5">
+        <f>MAX(GEOMEAN(J4:L4)-$B$38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <f>$H4*V4</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <f>MAX(0,$B$38-GEOMEAN(J4:L4))</f>
+        <v>10.619332496528237</v>
+      </c>
+      <c r="Y4" s="5">
+        <f>$H4*X4</f>
+        <v>0.15928973870557805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1374,59 +1846,91 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E30" si="0">COUNTIF(B5:D5,2)</f>
+        <f t="shared" ref="E5:E30" si="5">COUNTIF(B5:D5,2)</f>
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F30" si="1">COUNTIF(B5:D5,1)</f>
+        <f t="shared" ref="F5:F30" si="6">COUNTIF(B5:D5,1)</f>
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ref="G5:G32" si="2">COUNTIF(B5:D5,0)</f>
+        <f t="shared" ref="G5:G30" si="7">COUNTIF(B5:D5,0)</f>
         <v>2</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H30" si="3">($B$44^E5)*($B$45^G5)*($B$46^F5)</f>
-        <v>3.9602063250734842E-2</v>
+        <f t="shared" ref="H5:H30" si="8">($B$44^E5)*($B$45^G5)*($B$46^F5)</f>
+        <v>3.0408162487267697E-2</v>
       </c>
       <c r="I5" s="1">
-        <f>$B$34</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" ref="J5:J30" si="4">I5*EXP((B5-1)*$B$41)</f>
+        <f t="shared" ref="J5:J30" si="9">I5*EXP((B5-1)*$B$41)</f>
         <v>23.482334319742424</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" ref="K5:K30" si="5">J5*EXP((C5-1)*$B$41)</f>
+        <f t="shared" ref="K5:K30" si="10">J5*EXP((C5-1)*$B$41)</f>
         <v>18.380667503471763</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" ref="L5:L30" si="6">K5*EXP((D5-1)*$B$41)</f>
+        <f t="shared" ref="L5:L30" si="11">K5*EXP((D5-1)*$B$41)</f>
         <v>18.380667503471763</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" ref="M5:M30" si="7">AVERAGE(J5:L5)</f>
+        <f t="shared" ref="M5:M30" si="12">AVERAGE(J5:L5)</f>
         <v>20.081223108895319</v>
       </c>
       <c r="N5" s="2">
-        <f>MAX(L5-$B$38, 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f>$H5*N5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P5" s="2">
-        <f>MAX(0,$B$38-L5)</f>
+        <f t="shared" si="3"/>
         <v>10.619332496528237</v>
       </c>
       <c r="Q5" s="2">
-        <f>$H5*P5</f>
-        <v>0.42054747720809521</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.32291438806075279</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" ref="R5:R30" si="13">MAX(AVERAGE(J5:L5)-$B$38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" ref="S5:S30" si="14">$H5*R5</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" ref="T5:T30" si="15">MAX(0,$B$38-M5)</f>
+        <v>8.918776891104681</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" ref="U5:U30" si="16">$H5*T5</f>
+        <v>0.27120361689239936</v>
+      </c>
+      <c r="V5" s="5">
+        <f t="shared" ref="V5:V30" si="17">MAX(GEOMEAN(J5:L5)-$B$38, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
+        <f t="shared" ref="W5:W30" si="18">$H5*V5</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="5">
+        <f t="shared" ref="X5:X30" si="19">MAX(0,$B$38-GEOMEAN(J5:L5))</f>
+        <v>9.0555862578864819</v>
+      </c>
+      <c r="Y5" s="5">
+        <f t="shared" ref="Y5:Y30" si="20">$H5*X5</f>
+        <v>0.27536373834728056</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1440,59 +1944,91 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="8"/>
+        <v>1.5413817573457967E-2</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="10"/>
+        <v>18.380667503471763</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="11"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="12"/>
+        <v>21.781778714318872</v>
+      </c>
+      <c r="N6" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="1">
+      <c r="O6" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
         <f t="shared" si="3"/>
-        <v>1.7656844503188451E-2</v>
-      </c>
-      <c r="I6" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J6" s="1">
+        <v>5.5176656802575756</v>
+      </c>
+      <c r="Q6" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="5"/>
-        <v>18.380667503471763</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="6"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="M6" s="1">
-        <f t="shared" si="7"/>
-        <v>21.781778714318872</v>
-      </c>
-      <c r="N6" s="2">
-        <f>MAX(L6-$B$38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <f>$H6*N6</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <f>MAX(0,$B$38-L6)</f>
-        <v>5.5176656802575756</v>
-      </c>
-      <c r="Q6" s="2">
-        <f>$H6*P6</f>
-        <v>9.7424564936887531E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>8.504829222682013E-2</v>
+      </c>
+      <c r="R6" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="15"/>
+        <v>7.2182212856811283</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="16"/>
+        <v>0.11126034610234013</v>
+      </c>
+      <c r="V6" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="5">
+        <f t="shared" si="19"/>
+        <v>7.3588033763478187</v>
+      </c>
+      <c r="Y6" s="5">
+        <f t="shared" si="20"/>
+        <v>0.11342725280197183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1506,59 +2042,91 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="8"/>
+        <v>3.0408162487267697E-2</v>
+      </c>
+      <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="10"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="11"/>
+        <v>18.380667503471763</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="12"/>
+        <v>21.781778714318872</v>
+      </c>
+      <c r="N7" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="3"/>
-        <v>3.9602063250734842E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J7" s="1">
+        <v>10.619332496528237</v>
+      </c>
+      <c r="Q7" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="5"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="6"/>
-        <v>18.380667503471763</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" si="7"/>
-        <v>21.781778714318872</v>
-      </c>
-      <c r="N7" s="2">
-        <f>MAX(L7-$B$38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
-        <f>$H7*N7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <f>MAX(0,$B$38-L7)</f>
-        <v>10.619332496528237</v>
-      </c>
-      <c r="Q7" s="2">
-        <f>$H7*P7</f>
-        <v>0.42054747720809521</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.32291438806075279</v>
+      </c>
+      <c r="R7" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="15"/>
+        <v>7.2182212856811283</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="16"/>
+        <v>0.21949284572404609</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="5">
+        <f t="shared" si="19"/>
+        <v>7.3588033763478151</v>
+      </c>
+      <c r="Y7" s="5">
+        <f t="shared" si="20"/>
+        <v>0.22376768877983852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1572,59 +2140,91 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="8"/>
+        <v>6.1643852651282756E-2</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="10"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="11"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="12"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="N8" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="3"/>
-        <v>6.9568026931060817E-2</v>
-      </c>
-      <c r="I8" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J8" s="1">
+        <v>5.5176656802575756</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="5"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="6"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="7"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="N8" s="2">
-        <f>MAX(L8-$B$38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <f>$H8*N8</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="2">
-        <f>MAX(0,$B$38-L8)</f>
+        <v>0.34013017017283781</v>
+      </c>
+      <c r="R8" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="15"/>
         <v>5.5176656802575756</v>
       </c>
-      <c r="Q8" s="2">
-        <f>$H8*P8</f>
-        <v>0.383853114640749</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U8" s="4">
+        <f t="shared" si="16"/>
+        <v>0.34013017017283781</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="5">
+        <f t="shared" si="19"/>
+        <v>5.5176656802575756</v>
+      </c>
+      <c r="Y8" s="5">
+        <f t="shared" si="20"/>
+        <v>0.34013017017283781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1638,59 +2238,91 @@
         <v>2</v>
       </c>
       <c r="E9" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
+      </c>
+      <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
+        <v>30</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="10"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="12"/>
+        <v>25.654889546494946</v>
+      </c>
+      <c r="N9" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="O9" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
+        <v>3.1247106749375048E-2</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="5"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="M9" s="1">
-        <f t="shared" si="7"/>
-        <v>25.654889546494946</v>
-      </c>
-      <c r="N9" s="2">
-        <f>MAX(L9-$B$38, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="O9" s="2">
-        <f>$H9*N9</f>
-        <v>3.1017369628906256E-2</v>
-      </c>
-      <c r="P9" s="2">
-        <f>MAX(0,$B$38-L9)</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
-        <f>$H9*P9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="15"/>
+        <v>3.345110453505054</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="16"/>
+        <v>0.1045250234291228</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="5">
+        <f t="shared" si="19"/>
+        <v>3.519892097764469</v>
+      </c>
+      <c r="Y9" s="5">
+        <f t="shared" si="20"/>
+        <v>0.10998644412512804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1704,59 +2336,91 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="8"/>
+        <v>1.5413817573457967E-2</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="11"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="12"/>
+        <v>25.654889546494946</v>
+      </c>
+      <c r="N10" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="1">
+      <c r="O10" s="2">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
         <f t="shared" si="3"/>
-        <v>1.7656844503188451E-2</v>
-      </c>
-      <c r="I10" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J10" s="1">
+        <v>5.5176656802575756</v>
+      </c>
+      <c r="Q10" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K10" s="1">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="6"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="M10" s="1">
-        <f t="shared" si="7"/>
-        <v>25.654889546494946</v>
-      </c>
-      <c r="N10" s="2">
-        <f>MAX(L10-$B$38, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <f>$H10*N10</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <f>MAX(0,$B$38-L10)</f>
-        <v>5.5176656802575756</v>
-      </c>
-      <c r="Q10" s="2">
-        <f>$H10*P10</f>
-        <v>9.7424564936887531E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>8.504829222682013E-2</v>
+      </c>
+      <c r="R10" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="15"/>
+        <v>3.345110453505054</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="16"/>
+        <v>5.1560922293394151E-2</v>
+      </c>
+      <c r="V10" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <f t="shared" si="19"/>
+        <v>3.5198920977644725</v>
+      </c>
+      <c r="Y10" s="5">
+        <f t="shared" si="20"/>
+        <v>5.4254974673197856E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1770,59 +2434,91 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
+      </c>
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="9"/>
+        <v>23.482334319742424</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="12"/>
+        <v>27.827444773247475</v>
+      </c>
+      <c r="N11" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="O11" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
+        <v>3.1247106749375048E-2</v>
+      </c>
+      <c r="P11" s="2">
         <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
-      </c>
-      <c r="I11" s="1">
-        <f>$B$34</f>
-        <v>30</v>
-      </c>
-      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
         <f t="shared" si="4"/>
-        <v>23.482334319742424</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="M11" s="1">
-        <f t="shared" si="7"/>
-        <v>27.827444773247475</v>
-      </c>
-      <c r="N11" s="2">
-        <f>MAX(L11-$B$38, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="O11" s="2">
-        <f>$H11*N11</f>
-        <v>3.1017369628906256E-2</v>
-      </c>
-      <c r="P11" s="2">
-        <f>MAX(0,$B$38-L11)</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <f>$H11*P11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="15"/>
+        <v>1.1725552267525252</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="16"/>
+        <v>3.6638958339873823E-2</v>
+      </c>
+      <c r="V11" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="5">
+        <f t="shared" si="19"/>
+        <v>1.3521567375126722</v>
+      </c>
+      <c r="Y11" s="5">
+        <f t="shared" si="20"/>
+        <v>4.2250985918945168E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1836,59 +2532,91 @@
         <v>2</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="3"/>
-        <v>1.3829301492905311E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5839076213003733E-2</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" ref="I12:I30" si="8">$B$34</f>
+        <f t="shared" ref="I12:I30" si="21">$B$34</f>
         <v>30</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>23.482334319742424</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>30.60300600643286</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" ref="N12:N30" si="9">MAX(L12-$B$38, 0)</f>
+        <f t="shared" ref="N12:N30" si="22">MAX(L12-$B$38, 0)</f>
         <v>9.3266836995561491</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" ref="O12:O30" si="10">$H12*N12</f>
-        <v>0.12898152081012748</v>
+        <f t="shared" ref="O12:O30" si="23">$H12*N12</f>
+        <v>0.14772605393184945</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" ref="P12:P30" si="11">MAX(0,$B$38-L12)</f>
+        <f t="shared" ref="P12:P30" si="24">MAX(0,$B$38-L12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" ref="Q12:Q30" si="12">$H12*P12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q12:Q30" si="25">$H12*P12</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" si="13"/>
+        <v>1.6030060064328602</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="14"/>
+        <v>2.5390134305792823E-2</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="5">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="W12" s="5">
+        <f t="shared" si="18"/>
+        <v>1.5839076213003733E-2</v>
+      </c>
+      <c r="X12" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1902,59 +2630,91 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="3"/>
-        <v>3.9602063250734842E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.0408162487267697E-2</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>23.482334319742424</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>18.380667503471763</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>23.954333941071393</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>10.619332496528237</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="12"/>
-        <v>0.42054747720809521</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0.32291438806075279</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="15"/>
+        <v>5.0456660589286066</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="16"/>
+        <v>0.1534294333763927</v>
+      </c>
+      <c r="V13" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="5">
+        <f t="shared" si="19"/>
+        <v>5.5176656802575792</v>
+      </c>
+      <c r="Y13" s="5">
+        <f t="shared" si="20"/>
+        <v>0.16778207455569291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1968,59 +2728,91 @@
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="3"/>
-        <v>6.9568026931060817E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.1643852651282756E-2</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>23.482334319742424</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>23.482334319742424</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>25.654889546494946</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P14" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>5.5176656802575756</v>
       </c>
       <c r="Q14" s="2">
-        <f t="shared" si="12"/>
-        <v>0.383853114640749</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0.34013017017283781</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="15"/>
+        <v>3.345110453505054</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="16"/>
+        <v>0.2062054958981312</v>
+      </c>
+      <c r="V14" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="5">
+        <f t="shared" si="19"/>
+        <v>3.5198920977644725</v>
+      </c>
+      <c r="Y14" s="5">
+        <f t="shared" si="20"/>
+        <v>0.21697970982300771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -2034,59 +2826,91 @@
         <v>2</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>23.482334319742424</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="M15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>27.827444773247475</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="10"/>
-        <v>3.1017369628906256E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.1247106749375048E-2</v>
       </c>
       <c r="P15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q15" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" si="15"/>
+        <v>1.1725552267525252</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="16"/>
+        <v>3.6638958339873823E-2</v>
+      </c>
+      <c r="V15" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="5">
+        <f t="shared" si="19"/>
+        <v>1.3521567375126722</v>
+      </c>
+      <c r="Y15" s="5">
+        <f t="shared" si="20"/>
+        <v>4.2250985918945168E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -2100,59 +2924,91 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="3"/>
-        <v>6.9568026931060817E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.1643852651282756E-2</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>23.482334319742424</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>27.827444773247475</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>5.5176656802575756</v>
       </c>
       <c r="Q16" s="2">
-        <f t="shared" si="12"/>
-        <v>0.383853114640749</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0.34013017017283781</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" si="15"/>
+        <v>1.1725552267525252</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="16"/>
+        <v>7.2280821623424099E-2</v>
+      </c>
+      <c r="V16" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="X16" s="5">
+        <f t="shared" si="19"/>
+        <v>1.3521567375126722</v>
+      </c>
+      <c r="Y16" s="5">
+        <f t="shared" si="20"/>
+        <v>8.3352150688670384E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -2166,59 +3022,91 @@
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="3"/>
-        <v>0.12220854101562498</v>
+        <f t="shared" si="8"/>
+        <v>0.1249652809926991</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="10"/>
-        <v>0.12220854101562498</v>
+        <f t="shared" si="23"/>
+        <v>0.1249652809926991</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="14"/>
+        <v>0.1249652809926991</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="W17" s="5">
+        <f t="shared" si="18"/>
+        <v>0.1249652809926991</v>
+      </c>
+      <c r="X17" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -2232,59 +3120,91 @@
         <v>2</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="3"/>
-        <v>5.4487494553314177E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.3344572203068855E-2</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>32.775561233185385</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>9.3266836995561491</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="10"/>
-        <v>0.50818762728004974</v>
+        <f t="shared" si="23"/>
+        <v>0.59079478902171978</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <f t="shared" si="13"/>
+        <v>3.7755612331853854</v>
+      </c>
+      <c r="S18" s="4">
+        <f t="shared" si="14"/>
+        <v>0.23916131114261932</v>
+      </c>
+      <c r="T18" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="5">
+        <f t="shared" si="17"/>
+        <v>3.5522678733180797</v>
+      </c>
+      <c r="W18" s="5">
+        <f t="shared" si="18"/>
+        <v>0.22501688878603895</v>
+      </c>
+      <c r="X18" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -2298,59 +3218,91 @@
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>29.999999999999996</v>
       </c>
       <c r="M19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>32.775561233185385</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0.99999999999999645</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="10"/>
-        <v>3.1017369628906145E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.1247106749374937E-2</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" si="13"/>
+        <v>3.7755612331853854</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="14"/>
+        <v>0.11797536489214584</v>
+      </c>
+      <c r="T19" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="5">
+        <f t="shared" si="17"/>
+        <v>3.5522678733180797</v>
+      </c>
+      <c r="W19" s="5">
+        <f t="shared" si="18"/>
+        <v>0.11099809343994552</v>
+      </c>
+      <c r="X19" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2364,59 +3316,91 @@
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="3"/>
-        <v>5.4487494553314177E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.3344572203068855E-2</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>35.551122466370771</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>9.3266836995561491</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="10"/>
-        <v>0.50818762728004974</v>
+        <f t="shared" si="23"/>
+        <v>0.59079478902171978</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" si="13"/>
+        <v>6.5511224663707708</v>
+      </c>
+      <c r="S20" s="4">
+        <f t="shared" si="14"/>
+        <v>0.41497805008216981</v>
+      </c>
+      <c r="T20" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="5">
+        <f t="shared" si="17"/>
+        <v>6.3216714565418783</v>
+      </c>
+      <c r="W20" s="5">
+        <f t="shared" si="18"/>
+        <v>0.40044357402299646</v>
+      </c>
+      <c r="X20" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2430,59 +3414,91 @@
         <v>2</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4293613507077674E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2109197016283501E-2</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>48.964489446860775</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>39.09705771547231</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>19.964489446860775</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="10"/>
-        <v>0.48500959048816661</v>
+        <f t="shared" si="23"/>
+        <v>0.64104372497876538</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="13"/>
+        <v>10.09705771547231</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="14"/>
+        <v>0.3242084154708858</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="5">
+        <f t="shared" si="17"/>
+        <v>9.3266836995561491</v>
+      </c>
+      <c r="W21" s="5">
+        <f t="shared" si="18"/>
+        <v>0.29947232441760829</v>
+      </c>
+      <c r="X21" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -2496,59 +3512,91 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="3"/>
-        <v>1.7656844503188451E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5413817573457967E-2</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>29.999999999999996</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>23.482334319742421</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>30.603006006432853</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>5.5176656802575792</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="12"/>
-        <v>9.74245649368876E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>8.5048292226820185E-2</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" si="13"/>
+        <v>1.6030060064328531</v>
+      </c>
+      <c r="S22" s="4">
+        <f t="shared" si="14"/>
+        <v>2.4708442152313385E-2</v>
+      </c>
+      <c r="T22" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="5">
+        <f t="shared" si="17"/>
+        <v>0.99999999999999645</v>
+      </c>
+      <c r="W22" s="5">
+        <f t="shared" si="18"/>
+        <v>1.5413817573457911E-2</v>
+      </c>
+      <c r="X22" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -2562,59 +3610,91 @@
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>29.999999999999996</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>29.999999999999996</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>32.775561233185378</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0.99999999999999645</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="10"/>
-        <v>3.1017369628906145E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.1247106749374937E-2</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q23" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" si="13"/>
+        <v>3.7755612331853783</v>
+      </c>
+      <c r="S23" s="4">
+        <f t="shared" si="14"/>
+        <v>0.11797536489214562</v>
+      </c>
+      <c r="T23" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="5">
+        <f t="shared" si="17"/>
+        <v>3.5522678733180797</v>
+      </c>
+      <c r="W23" s="5">
+        <f t="shared" si="18"/>
+        <v>0.11099809343994552</v>
+      </c>
+      <c r="X23" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -2628,59 +3708,91 @@
         <v>2</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="3"/>
-        <v>1.3829301492905311E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5839076213003733E-2</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>29.999999999999996</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>35.551122466370764</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>9.3266836995561491</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="10"/>
-        <v>0.12898152081012748</v>
+        <f t="shared" si="23"/>
+        <v>0.14772605393184945</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="4">
+        <f t="shared" si="13"/>
+        <v>6.5511224663707637</v>
+      </c>
+      <c r="S24" s="4">
+        <f t="shared" si="14"/>
+        <v>0.10376372802556751</v>
+      </c>
+      <c r="T24" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="5">
+        <f t="shared" si="17"/>
+        <v>6.3216714565418783</v>
+      </c>
+      <c r="W24" s="5">
+        <f t="shared" si="18"/>
+        <v>0.10012943599373712</v>
+      </c>
+      <c r="X24" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -2694,59 +3806,91 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="3"/>
-        <v>3.1017369628906256E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1247106749375048E-2</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>29.999999999999996</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>35.551122466370764</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0.99999999999999645</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="10"/>
-        <v>3.1017369628906145E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.1247106749374937E-2</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q25" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" si="13"/>
+        <v>6.5511224663707637</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="14"/>
+        <v>0.2047036230349164</v>
+      </c>
+      <c r="T25" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="5">
+        <f t="shared" si="17"/>
+        <v>6.3216714565418783</v>
+      </c>
+      <c r="W25" s="5">
+        <f t="shared" si="18"/>
+        <v>0.19753394283704132</v>
+      </c>
+      <c r="X25" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -2760,59 +3904,91 @@
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="3"/>
-        <v>5.4487494553314177E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.3344572203068855E-2</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>38.326683699556149</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>9.3266836995561491</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="10"/>
-        <v>0.50818762728004974</v>
+        <f t="shared" si="23"/>
+        <v>0.59079478902171978</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="4">
+        <f t="shared" si="13"/>
+        <v>9.3266836995561491</v>
+      </c>
+      <c r="S26" s="4">
+        <f t="shared" si="14"/>
+        <v>0.59079478902171978</v>
+      </c>
+      <c r="T26" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="5">
+        <f t="shared" si="17"/>
+        <v>9.3266836995561491</v>
+      </c>
+      <c r="W26" s="5">
+        <f t="shared" si="18"/>
+        <v>0.59079478902171978</v>
+      </c>
+      <c r="X26" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -2826,59 +4002,91 @@
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4293613507077674E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2109197016283501E-2</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>38.326683699556149</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>48.964489446860775</v>
       </c>
       <c r="M27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>41.872618948657696</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>19.964489446860775</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="10"/>
-        <v>0.48500959048816661</v>
+        <f t="shared" si="23"/>
+        <v>0.64104372497876538</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q27" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="4">
+        <f t="shared" si="13"/>
+        <v>12.872618948657696</v>
+      </c>
+      <c r="S27" s="4">
+        <f t="shared" si="14"/>
+        <v>0.41332945793799414</v>
+      </c>
+      <c r="T27" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="5">
+        <f t="shared" si="17"/>
+        <v>12.587349149462845</v>
+      </c>
+      <c r="W27" s="5">
+        <f t="shared" si="18"/>
+        <v>0.40416967375285107</v>
+      </c>
+      <c r="X27" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -2892,59 +4100,91 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="3"/>
-        <v>1.3829301492905311E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5839076213003733E-2</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>48.964489446860775</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>38.326683699556149</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>41.872618948657696</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>9.3266836995561491</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="10"/>
-        <v>0.12898152081012748</v>
+        <f t="shared" si="23"/>
+        <v>0.14772605393184945</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q28" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="13"/>
+        <v>12.872618948657696</v>
+      </c>
+      <c r="S28" s="4">
+        <f t="shared" si="14"/>
+        <v>0.20389039258874522</v>
+      </c>
+      <c r="T28" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="5">
+        <f t="shared" si="17"/>
+        <v>12.587349149462845</v>
+      </c>
+      <c r="W28" s="5">
+        <f t="shared" si="18"/>
+        <v>0.19937198249802973</v>
+      </c>
+      <c r="X28" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -2958,59 +4198,91 @@
         <v>1</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4293613507077674E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2109197016283501E-2</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>48.964489446860775</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>48.964489446860775</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>45.418554197759228</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>19.964489446860775</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="10"/>
-        <v>0.48500959048816661</v>
+        <f t="shared" si="23"/>
+        <v>0.64104372497876538</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q29" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="4">
+        <f t="shared" si="13"/>
+        <v>16.418554197759228</v>
+      </c>
+      <c r="S29" s="4">
+        <f t="shared" si="14"/>
+        <v>0.52718659145837954</v>
+      </c>
+      <c r="T29" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="5">
+        <f t="shared" si="17"/>
+        <v>16.12541765515072</v>
+      </c>
+      <c r="W29" s="5">
+        <f t="shared" si="18"/>
+        <v>0.51777421245909083</v>
+      </c>
+      <c r="X29" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -3024,88 +4296,176 @@
         <v>2</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="3"/>
-        <v>1.0831469900929208E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.6276067501495579E-2</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>38.326683699556149</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>48.964489446860775</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>62.554883318002936</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>49.948685488139951</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>33.554883318002936</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="10"/>
-        <v>0.36344870868814039</v>
+        <f t="shared" si="23"/>
+        <v>0.54614154588862374</v>
       </c>
       <c r="P30" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q30" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="4">
+        <f t="shared" si="13"/>
+        <v>20.948685488139951</v>
+      </c>
+      <c r="S30" s="4">
+        <f t="shared" si="14"/>
+        <v>0.34096221907256669</v>
+      </c>
+      <c r="T30" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="5">
+        <f t="shared" si="17"/>
+        <v>19.964489446860775</v>
+      </c>
+      <c r="W30" s="5">
+        <f t="shared" si="18"/>
+        <v>0.3249433778700021</v>
+      </c>
+      <c r="X30" s="5">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="5">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="O31" s="2">
         <f>SUM(O4:O30)</f>
-        <v>4.0382976832122335</v>
+        <v>4.9972831711745771</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="Q31" s="2">
         <f>SUM(Q4:Q30)</f>
-        <v>3.0348988719385646</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2.4634677194333592</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S31" s="4">
+        <f>SUM(S4:S30)</f>
+        <v>3.7739931650706611</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U31" s="4">
+        <f>SUM(U4:U30)</f>
+        <v>1.7571145130979404</v>
+      </c>
+      <c r="V31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W31" s="5">
+        <f>SUM(W4:W30)</f>
+        <v>3.6378645633181672</v>
+      </c>
+      <c r="X31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y31" s="5">
+        <f>SUM(Y4:Y30)</f>
+        <v>1.8288359145110942</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="O32" s="2">
         <f>O31/((1+$B$36)^3)</f>
-        <v>4.0382976832122335</v>
+        <v>4.3168410937692059</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="Q32" s="2">
         <f>Q31/((1+$B$36)^3)</f>
-        <v>3.0348988719385646</v>
+        <v>2.1280360388151247</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" s="4">
+        <f>S31/((1+$B$36)^3)</f>
+        <v>3.2601171925888441</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U32" s="4">
+        <f>U31/((1+$B$36)^3)</f>
+        <v>1.5178615813393286</v>
+      </c>
+      <c r="V32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W32" s="5">
+        <f>W31/((1+$B$36)^3)</f>
+        <v>3.1425241881595221</v>
+      </c>
+      <c r="X32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y32" s="5">
+        <f>Y31/((1+$B$36)^3)</f>
+        <v>1.5798172244993793</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3130,7 +4490,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3177,7 +4537,7 @@
       </c>
       <c r="B42" s="3">
         <f>B36-(0.5*B35*B35)</f>
-        <v>-4.4999999999999998E-2</v>
+        <v>5.0000000000000044E-3</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3190,7 +4550,7 @@
       </c>
       <c r="B44" s="3">
         <f>(((B35*B35*B40)+(B42*B42*B40*B40))/(B41*B41)+(B42*B40)/B41)/2</f>
-        <v>0.2212563782152103</v>
+        <v>0.253425217235347</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3199,7 +4559,7 @@
       </c>
       <c r="B45" s="3">
         <f>(((B35*B35*B40)+(B42*B42*B40*B40))/(B41*B41)-(B42*B40)/B41)/2</f>
-        <v>0.28249362178478976</v>
+        <v>0.24662107906094927</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3208,7 +4568,7 @@
       </c>
       <c r="B46" s="3">
         <f>1-B44-B45</f>
-        <v>0.49624999999999997</v>
+        <v>0.49995370370370368</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>